<commit_message>
corrected ref designator for WFP03
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="69">
   <si>
     <t>Ref Des</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>GS02HYPM-WFP02-00-WFPENG000</t>
+  </si>
+  <si>
+    <t>GS02HYPM-WFP03-00-WFPENG000</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2318,7 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Corrections to reference designators, added controller to integration
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="71">
   <si>
     <t>Ref Des</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>89° 22.1060' W</t>
-  </si>
-  <si>
-    <t>GS02HYPM-MFC04-01-ZPLSGA000 unit not deployed</t>
   </si>
   <si>
     <t>GS02HYPM</t>
@@ -260,6 +257,15 @@
   </si>
   <si>
     <t>GS02HYPM-WFP03-00-WFPENG000</t>
+  </si>
+  <si>
+    <t>GS02HYPM-MPM01-02-ZPLSGA009</t>
+  </si>
+  <si>
+    <t>GS02HYPM-MPM01-02-ZPLSGA010</t>
+  </si>
+  <si>
+    <t>Not Deployed</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>0</v>
@@ -1275,10 +1281,10 @@
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>30</v>
@@ -1305,7 +1311,7 @@
         <v>4650</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="12">
@@ -1371,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1393,7 @@
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -1396,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>1</v>
@@ -1405,7 +1411,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>2</v>
@@ -1426,7 +1432,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
@@ -1435,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1">
         <v>3281</v>
@@ -1455,7 +1461,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -1464,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1">
         <v>3281</v>
@@ -1481,7 +1487,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -1490,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1">
         <v>3281</v>
@@ -1507,7 +1513,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -1516,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1">
         <v>3281</v>
@@ -1533,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -1542,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1">
         <v>3281</v>
@@ -1562,7 +1568,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -1571,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1">
         <v>3281</v>
@@ -1591,7 +1597,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -1600,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1">
         <v>3281</v>
@@ -1620,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -1629,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1">
         <v>3281</v>
@@ -1649,7 +1655,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
@@ -1658,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1">
         <v>1477</v>
@@ -1678,7 +1684,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1687,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>1477</v>
@@ -1704,7 +1710,7 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -1713,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="1">
         <v>133</v>
@@ -1730,7 +1736,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
@@ -1739,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1">
         <v>133</v>
@@ -1756,7 +1762,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -1765,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1">
         <v>1116</v>
@@ -1782,7 +1788,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -1791,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1">
         <v>1116</v>
@@ -1808,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
@@ -1817,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1">
         <v>3282</v>
@@ -1837,7 +1843,7 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
@@ -1846,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1">
         <v>3282</v>
@@ -1863,7 +1869,7 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -1872,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="1">
         <v>3282</v>
@@ -1889,7 +1895,7 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -1898,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="1">
         <v>3282</v>
@@ -1915,7 +1921,7 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -1924,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="1">
         <v>3282</v>
@@ -1944,7 +1950,7 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -1953,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="1">
         <v>3282</v>
@@ -1973,7 +1979,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
@@ -1982,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1">
         <v>3282</v>
@@ -2002,7 +2008,7 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>30</v>
@@ -2011,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="1">
         <v>3282</v>
@@ -2031,7 +2037,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -2040,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="1">
         <v>1479</v>
@@ -2057,7 +2063,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -2066,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="20">
         <v>1479</v>
@@ -2083,7 +2089,7 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>30</v>
@@ -2092,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F33" s="1">
         <v>130</v>
@@ -2109,7 +2115,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>30</v>
@@ -2118,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F34" s="1">
         <v>130</v>
@@ -2135,7 +2141,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>30</v>
@@ -2144,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F36" s="1">
         <v>1118</v>
@@ -2161,7 +2167,7 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>30</v>
@@ -2170,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F37" s="1">
         <v>1118</v>
@@ -2182,17 +2188,29 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
       <c r="I39" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>63</v>
+      <c r="A41" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>30</v>
@@ -2200,51 +2218,16 @@
       <c r="D41" s="1">
         <v>1</v>
       </c>
-      <c r="E41" t="s">
-        <v>60</v>
-      </c>
-      <c r="F41" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="1">
-        <v>-54.468344999999999</v>
+      <c r="I41" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>30</v>
@@ -2253,89 +2236,141 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F43" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>59</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="1">
-        <v>-89.368433333333329</v>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-54.468344999999999</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-89.368433333333329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B45" t="s">
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="B48"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="18"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="18"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="I49" s="18"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>61</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F50" t="s">
         <v>49</v>
       </c>
-      <c r="I47" s="18"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" s="18"/>
+      <c r="I50" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to Southern Ocean CTDMO calibration coefficients
The following calibration coefficients added to all Southern Ocean
CTDMOs per Redmine ticket 10208. Updates made by Rebecca Travis.

CC_wbotc
CC_a0
CC_a1
CC_a2
CC_a3
CC_ptempa0
CC_ptempa1
CC_ptempa2
CC_ptca0
CC_ptca1
CC_ptca2
CC_ptcb0
CC_ptcb1
CC_ptcb2
CC_pa0
CC_pa1
CC_pa2
CC_g
CC_h
CC_i
CC_j
CC_cpcor
CC_ctcor
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS02HYPM_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtravis\Desktop\Cal Sheet project\SO_cal_sheets_RT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25000" windowHeight="13980" activeTab="1"/>
+    <workbookView xWindow="36" yWindow="0" windowWidth="24996" windowHeight="13980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="96">
   <si>
     <t>Ref Des</t>
   </si>
@@ -262,18 +267,94 @@
   <si>
     <t>Not Deployed</t>
   </si>
+  <si>
+    <t>Induction ID</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>CC_wbotc</t>
+  </si>
+  <si>
+    <t>CC_a0</t>
+  </si>
+  <si>
+    <t>CC_a1</t>
+  </si>
+  <si>
+    <t>CC_a2</t>
+  </si>
+  <si>
+    <t>CC_a3</t>
+  </si>
+  <si>
+    <t>CC_ptempa0</t>
+  </si>
+  <si>
+    <t>CC_ptempa1</t>
+  </si>
+  <si>
+    <t>CC_ptempa2</t>
+  </si>
+  <si>
+    <t>CC_ptca0</t>
+  </si>
+  <si>
+    <t>CC_ptca1</t>
+  </si>
+  <si>
+    <t>CC_ptca2</t>
+  </si>
+  <si>
+    <t>CC_ptcb0</t>
+  </si>
+  <si>
+    <t>CC_ptcb1</t>
+  </si>
+  <si>
+    <t>CC_ptcb2</t>
+  </si>
+  <si>
+    <t>CC_pa0</t>
+  </si>
+  <si>
+    <t>CC_pa1</t>
+  </si>
+  <si>
+    <t>CC_pa2</t>
+  </si>
+  <si>
+    <t>CC_g</t>
+  </si>
+  <si>
+    <t>CC_h</t>
+  </si>
+  <si>
+    <t>CC_i</t>
+  </si>
+  <si>
+    <t>CC_j</t>
+  </si>
+  <si>
+    <t>CC_cpcor</t>
+  </si>
+  <si>
+    <t>CC_ctcor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,8 +541,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +588,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,7 +783,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -757,6 +857,36 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="29" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="133">
@@ -908,7 +1038,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1217,26 +1347,26 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" style="3" customWidth="1"/>
     <col min="15" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>45</v>
       </c>
@@ -1274,7 +1404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1318,43 +1448,43 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1"/>
-    <row r="5" spans="1:14" s="8" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:14" s="8" customFormat="1">
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E6" s="13"/>
       <c r="F6" s="14"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:14" s="8" customFormat="1">
+    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1">
+    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:14" s="8" customFormat="1">
+    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:14" s="8" customFormat="1">
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1">
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -1372,27 +1502,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="24" customFormat="1" ht="28">
+    <row r="1" spans="1:9" s="24" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1421,8 +1551,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1"/>
-    <row r="3" spans="1:9">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1451,7 +1581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1477,7 +1607,7 @@
         <v>1.725E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1503,7 +1633,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1529,7 +1659,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1558,7 +1688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1587,7 +1717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1616,7 +1746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1645,7 +1775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1674,7 +1804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1700,7 +1830,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1726,7 +1856,7 @@
         <v>-54.468344999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1882,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1778,7 +1908,7 @@
         <v>-54.468344999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1804,7 +1934,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1833,7 +1963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1859,7 +1989,7 @@
         <v>1.6920000000000001E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1885,7 +2015,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +2041,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1940,7 +2070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1969,7 +2099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1998,7 +2128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -2027,7 +2157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -2053,7 +2183,7 @@
         <v>-54.468344999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -2079,7 +2209,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2105,7 +2235,7 @@
         <v>-54.468344999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -2131,7 +2261,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2157,7 +2287,7 @@
         <v>-54.468344999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -2183,7 +2313,7 @@
         <v>-89.368433333333329</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
@@ -2200,7 +2330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
@@ -2217,7 +2347,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -2236,136 +2366,795 @@
       <c r="F43" t="s">
         <v>58</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H43" s="27">
+        <v>42</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="28">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="35">
+        <v>1</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="29">
+        <v>-54.468344999999999</v>
+      </c>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="35">
+        <v>1</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="29">
+        <v>-89.368433333333329</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="35">
+        <v>1</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H46" s="27">
         <v>1450</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B47" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="35">
+        <v>1</v>
+      </c>
+      <c r="E47" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F47" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="1">
-        <v>-54.468344999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
+      <c r="G47" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H47" s="33">
+        <v>6.7578000000000003E-7</v>
+      </c>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B48" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="35">
+        <v>1</v>
+      </c>
+      <c r="E48" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F48" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="1">
-        <v>-89.368433333333329</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
+      <c r="G48" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="H48" s="34">
+        <v>-9.7107839999999995E-5</v>
+      </c>
+      <c r="I48" s="32"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="35">
+        <v>1</v>
+      </c>
+      <c r="E49" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="34">
+        <v>3.0705339999999998E-4</v>
+      </c>
+      <c r="I49" s="32"/>
+    </row>
+    <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="35">
+        <v>1</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G50" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="H50" s="34">
+        <v>-4.5325649999999997E-6</v>
+      </c>
+      <c r="I50" s="32"/>
+    </row>
+    <row r="51" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="35">
+        <v>1</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" s="34">
+        <v>2.0306339999999999E-7</v>
+      </c>
+      <c r="I51" s="32"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="35">
+        <v>1</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="33">
+        <v>-70.188689999999994</v>
+      </c>
+      <c r="I52" s="32"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="35">
+        <v>1</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H53" s="33">
+        <v>5.0994060000000001E-2</v>
+      </c>
+      <c r="I53" s="32"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="35">
+        <v>1</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="H54" s="33">
+        <v>-3.8153629999999999E-7</v>
+      </c>
+      <c r="I54" s="32"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="35">
+        <v>1</v>
+      </c>
+      <c r="E55" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G55" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="H55" s="33">
+        <v>524846.6</v>
+      </c>
+      <c r="I55" s="32"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="35">
+        <v>1</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="H56" s="33">
+        <v>3.312093</v>
+      </c>
+      <c r="I56" s="32"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="35">
+        <v>1</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G57" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H57" s="33">
+        <v>-7.3581999999999996E-3</v>
+      </c>
+      <c r="I57" s="32"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="35">
+        <v>1</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H58" s="33">
+        <v>25.37125</v>
+      </c>
+      <c r="I58" s="32"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="35">
+        <v>1</v>
+      </c>
+      <c r="E59" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="H59" s="33">
+        <v>-1.4999999999999999E-4</v>
+      </c>
+      <c r="I59" s="32"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="35">
+        <v>1</v>
+      </c>
+      <c r="E60" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="H60" s="33">
+        <v>0</v>
+      </c>
+      <c r="I60" s="32"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="35">
+        <v>1</v>
+      </c>
+      <c r="E61" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H61" s="34">
+        <v>0.33191749999999998</v>
+      </c>
+      <c r="I61" s="32"/>
+    </row>
+    <row r="62" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="35">
+        <v>1</v>
+      </c>
+      <c r="E62" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" s="34">
+        <v>4.4613919999999998E-3</v>
+      </c>
+      <c r="I62" s="32"/>
+    </row>
+    <row r="63" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="35">
+        <v>1</v>
+      </c>
+      <c r="E63" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="H63" s="34">
+        <v>-1.03474E-11</v>
+      </c>
+      <c r="I63" s="32"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="35">
+        <v>1</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F64" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G64" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H64" s="33">
+        <v>-0.9834522</v>
+      </c>
+      <c r="I64" s="32"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="35">
+        <v>1</v>
+      </c>
+      <c r="E65" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F65" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="H65" s="33">
+        <v>0.14677190000000001</v>
+      </c>
+      <c r="I65" s="32"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="35">
+        <v>1</v>
+      </c>
+      <c r="E66" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F66" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="H66" s="33">
+        <v>-1.209564E-4</v>
+      </c>
+      <c r="I66" s="32"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="35">
+        <v>1</v>
+      </c>
+      <c r="E67" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F67" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G67" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="H67" s="33">
+        <v>3.1289630000000001E-5</v>
+      </c>
+      <c r="I67" s="32"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="35">
+        <v>1</v>
+      </c>
+      <c r="E68" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F68" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G68" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="H68" s="33">
+        <v>-9.5700000000000003E-8</v>
+      </c>
+      <c r="I68" s="32"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="35">
+        <v>1</v>
+      </c>
+      <c r="E69" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F69" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G69" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H69" s="33">
+        <v>3.2499999999999998E-6</v>
+      </c>
+      <c r="I69" s="32"/>
+    </row>
+    <row r="71" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>63</v>
       </c>
-      <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="16"/>
-      <c r="B48"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="18"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="16" t="s">
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="16"/>
+      <c r="B72"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="18"/>
+    </row>
+    <row r="73" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
         <v>60</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F73" t="s">
         <v>48</v>
       </c>
-      <c r="I49" s="18"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="16" t="s">
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B74" t="s">
+        <v>47</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
         <v>61</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F74" t="s">
         <v>49</v>
       </c>
-      <c r="I50" s="18"/>
+      <c r="I74" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>